<commit_message>
arregle el remove productos y tiendas
</commit_message>
<xml_diff>
--- a/ventas.xlsx
+++ b/ventas.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,12 +505,12 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>7702018913664</t>
+          <t>750107904444</t>
         </is>
       </c>
       <c r="B3" s="15" t="inlineStr">
         <is>
-          <t>desodorante gel-gillette</t>
+          <t>Crema Ponds</t>
         </is>
       </c>
       <c r="C3" s="15" t="inlineStr">
@@ -522,216 +522,216 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>750107904444</t>
+          <t>75007614</t>
         </is>
       </c>
       <c r="B4" s="15" t="inlineStr">
         <is>
-          <t>Crema Ponds</t>
+          <t xml:space="preserve">Coca cola </t>
         </is>
       </c>
       <c r="C4" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t xml:space="preserve">Mililitros </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>75007614</t>
+          <t>80741251</t>
         </is>
       </c>
       <c r="B5" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Coca cola </t>
+          <t>Kinder Sorpresa Niña</t>
         </is>
       </c>
       <c r="C5" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mililitros </t>
+          <t xml:space="preserve">Pieza </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>80741251</t>
+          <t>7501045403908</t>
         </is>
       </c>
       <c r="B6" s="15" t="inlineStr">
         <is>
-          <t>Kinder Sorpresa Niña</t>
+          <t xml:space="preserve">Atun Dolores Aceite </t>
         </is>
       </c>
       <c r="C6" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pieza </t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>750100912803</t>
+          <t>77910000031</t>
         </is>
       </c>
       <c r="B7" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nescafe </t>
+          <t>Cerillos Maya</t>
         </is>
       </c>
       <c r="C7" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>Cajas</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>7501045403908</t>
+          <t>7501020561906</t>
         </is>
       </c>
       <c r="B8" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Atun Dolores Aceite </t>
+          <t xml:space="preserve">Crema Lala </t>
         </is>
       </c>
       <c r="C8" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>Litros</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>97339000214</t>
+          <t>7501007704302</t>
         </is>
       </c>
       <c r="B9" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Valentina </t>
+          <t>Servilletas Pétalo</t>
         </is>
       </c>
       <c r="C9" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mililitros </t>
+          <t>Pieza</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>7506306245266</t>
+          <t>7501025412258</t>
         </is>
       </c>
       <c r="B10" s="15" t="inlineStr">
         <is>
-          <t>Ponds Hidra Active</t>
+          <t xml:space="preserve">Limpiador líquido Pinol </t>
         </is>
       </c>
       <c r="C10" s="15" t="inlineStr">
         <is>
-          <t>Mililitros</t>
+          <t>Litros</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>7501026004605</t>
+          <t>7501055367825</t>
         </is>
       </c>
       <c r="B11" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jabón Roma </t>
+          <t>leche santa clara de vainilla</t>
         </is>
       </c>
       <c r="C11" s="15" t="inlineStr">
         <is>
-          <t>Kilogramos</t>
+          <t>Mililitros</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>77910000031</t>
+          <t>7501011143586</t>
         </is>
       </c>
       <c r="B12" s="15" t="inlineStr">
         <is>
-          <t>Cerillos Maya</t>
+          <t>Chetos torciditos</t>
         </is>
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>Cajas</t>
+          <t xml:space="preserve">Gramos </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>7501020561906</t>
+          <t>7501031307210</t>
         </is>
       </c>
       <c r="B13" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Crema Lala </t>
+          <t>Jumex fresh de naranja</t>
         </is>
       </c>
       <c r="C13" s="15" t="inlineStr">
         <is>
-          <t>Litros</t>
+          <t>Mililitros</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>7501040090165</t>
+          <t>7509546059006</t>
         </is>
       </c>
       <c r="B14" s="15" t="inlineStr">
         <is>
-          <t>Yogurt Frutas y Cereales Yoplait</t>
+          <t>Fijador Palmolive Caprice 316 ml</t>
         </is>
       </c>
       <c r="C14" s="15" t="inlineStr">
         <is>
-          <t>Litros</t>
+          <t>Mililitros</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>7501007704302</t>
+          <t>7501052475011</t>
         </is>
       </c>
       <c r="B15" s="15" t="inlineStr">
         <is>
-          <t>Servilletas Pétalo</t>
+          <t>Vinagre Blanco Clemente Jacques 1L</t>
         </is>
       </c>
       <c r="C15" s="15" t="inlineStr">
         <is>
-          <t>Pieza</t>
+          <t>Litros</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>7501025412258</t>
+          <t>7501052475240</t>
         </is>
       </c>
       <c r="B16" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Limpiador líquido Pinol </t>
+          <t>Vinagre de Manzana Clemente Jacques 1L</t>
         </is>
       </c>
       <c r="C16" s="15" t="inlineStr">
@@ -743,369 +743,365 @@
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>7502261263529</t>
+          <t>7506475104722</t>
         </is>
       </c>
       <c r="B17" s="15" t="inlineStr">
         <is>
-          <t>Chocolate oscuro Lancelot</t>
+          <t>Leche Condensada Nestlé La Lechera Original 375g</t>
         </is>
       </c>
       <c r="C17" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gramos </t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>7501055367825</t>
+          <t>7501040009761</t>
         </is>
       </c>
       <c r="B18" s="15" t="inlineStr">
         <is>
-          <t>leche santa clara de vainilla</t>
+          <t>Salchicas FUD con pavo 266g</t>
         </is>
       </c>
       <c r="C18" s="15" t="inlineStr">
         <is>
-          <t>Mililitros</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>7501011143586</t>
+          <t>7501003340122</t>
         </is>
       </c>
       <c r="B19" s="15" t="inlineStr">
         <is>
-          <t>Chetos torciditos</t>
+          <t>Mayonesa McCormik 190g</t>
         </is>
       </c>
       <c r="C19" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gramos </t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>7502247427181</t>
+          <t>7503025355757</t>
         </is>
       </c>
       <c r="B20" s="15" t="inlineStr">
         <is>
-          <t>Chidas papas con sal</t>
+          <t>Arroz medio grano Cies 900g</t>
         </is>
       </c>
       <c r="C20" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gramos </t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>7501031307210</t>
+          <t>7501040090967</t>
         </is>
       </c>
       <c r="B21" s="15" t="inlineStr">
         <is>
-          <t>Jumex fresh de naranja</t>
+          <t>Yoghurt natural Yoplait 442g</t>
         </is>
       </c>
       <c r="C21" s="15" t="inlineStr">
         <is>
-          <t>Mililitros</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>7509546059006</t>
+          <t>7502261257856</t>
         </is>
       </c>
       <c r="B22" s="15" t="inlineStr">
         <is>
-          <t>Fijador Palmolive Caprice 316 ml</t>
+          <t>Crema blanca crema 450g</t>
         </is>
       </c>
       <c r="C22" s="15" t="inlineStr">
         <is>
-          <t>Mililitros</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>7501008019436</t>
+          <t>980022724</t>
         </is>
       </c>
       <c r="B23" s="15" t="inlineStr">
         <is>
-          <t>Choco Krispis 450g</t>
+          <t>Cajeta Quemada Member's Mark 1.2 k</t>
         </is>
       </c>
       <c r="C23" s="15" t="inlineStr">
         <is>
+          <t>kilogramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="16" t="inlineStr">
+        <is>
+          <t>-0-0-0931305</t>
+        </is>
+      </c>
+      <c r="B24" s="15" t="inlineStr">
+        <is>
+          <t>Frijol Verde Valle Flor de Mayo 2.5 kg</t>
+        </is>
+      </c>
+      <c r="C24" s="15" t="inlineStr">
+        <is>
+          <t>kilogramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="16" t="inlineStr">
+        <is>
+          <t>-0-0-0-358602</t>
+        </is>
+      </c>
+      <c r="B25" s="15" t="inlineStr">
+        <is>
+          <t>Polvo para Preparar Bebida Gatorade Rehidratante 2.38 kg</t>
+        </is>
+      </c>
+      <c r="C25" s="15" t="inlineStr">
+        <is>
+          <t>kilogramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="16" t="inlineStr">
+        <is>
+          <t>4760413</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DORITOS 5 - 10 /54 GRS PACK </t>
+        </is>
+      </c>
+      <c r="C26" s="15" t="inlineStr">
+        <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>7501058624147</t>
-        </is>
-      </c>
-      <c r="B24" s="15" t="inlineStr">
-        <is>
-          <t>NESCAFÉ Reserva Verarica 180g</t>
-        </is>
-      </c>
-      <c r="C24" s="15" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="16" t="inlineStr">
+        <is>
+          <t>9987980</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>MAXI BOTANA INTENSOS TOTIS 40-85GR</t>
+        </is>
+      </c>
+      <c r="C27" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>7501052475011</t>
-        </is>
-      </c>
-      <c r="B25" s="15" t="inlineStr">
-        <is>
-          <t>Vinagre Blanco Clemente Jacques 1L</t>
-        </is>
-      </c>
-      <c r="C25" s="15" t="inlineStr">
-        <is>
-          <t>Litros</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>7501052475240</t>
-        </is>
-      </c>
-      <c r="B26" s="15" t="inlineStr">
-        <is>
-          <t>Vinagre de Manzana Clemente Jacques 1L</t>
-        </is>
-      </c>
-      <c r="C26" s="15" t="inlineStr">
-        <is>
-          <t>Litros</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>7506475104722</t>
-        </is>
-      </c>
-      <c r="B27" s="15" t="inlineStr">
-        <is>
-          <t>Leche Condensada Nestlé La Lechera Original 375g</t>
-        </is>
-      </c>
-      <c r="C27" s="15" t="inlineStr">
+    <row r="28">
+      <c r="A28" s="16" t="inlineStr">
+        <is>
+          <t>9987979</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>BOTANA TOTOPOS NACHO TOTIS 40-120GR</t>
+        </is>
+      </c>
+      <c r="C28" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>7500478012404</t>
-        </is>
-      </c>
-      <c r="B28" s="15" t="inlineStr">
-        <is>
-          <t>Emperador Sabor Vainilla 36g</t>
-        </is>
-      </c>
-      <c r="C28" s="15" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="16" t="inlineStr">
+        <is>
+          <t>9987977</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>BOTANAS TOTIS TOP´S SALSA NEGRA 8-10/52 GR</t>
+        </is>
+      </c>
+      <c r="C29" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>7501055304653</t>
-        </is>
-      </c>
-      <c r="B29" s="15" t="inlineStr">
-        <is>
-          <t>Delaware punch sabor uva 600ml</t>
-        </is>
-      </c>
-      <c r="C29" s="15" t="inlineStr">
-        <is>
-          <t>Mililiros</t>
-        </is>
-      </c>
-    </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>7501000153374</t>
-        </is>
-      </c>
-      <c r="B30" s="15" t="inlineStr">
-        <is>
-          <t>Submarinos Marinela sabor fresa 105g</t>
+      <c r="A30" s="16" t="inlineStr">
+        <is>
+          <t>4760398</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="inlineStr">
+        <is>
+          <t>BOTANA DORITOS PACK 1-30 PZ</t>
         </is>
       </c>
       <c r="C30" s="15" t="inlineStr">
         <is>
+          <t>Pieza</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="16" t="inlineStr">
+        <is>
+          <t>4761205</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>BOTANA SABRISURTIDO SABRITAS 1-35 PZ</t>
+        </is>
+      </c>
+      <c r="C31" s="15" t="inlineStr">
+        <is>
+          <t>Piezas</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="16" t="inlineStr">
+        <is>
+          <t>4761234</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="inlineStr">
+        <is>
+          <t>BOTANA SABRIMAYOREO SABRITAS 1-50 PZ</t>
+        </is>
+      </c>
+      <c r="C32" s="15" t="inlineStr">
+        <is>
+          <t>Piezas</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="16" t="inlineStr">
+        <is>
+          <t>6307033</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>ACT II NATURAL OPTIMUS 6-14/80 GR (PALOMITAS)</t>
+        </is>
+      </c>
+      <c r="C33" s="15" t="inlineStr">
+        <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>7501045401423</t>
-        </is>
-      </c>
-      <c r="B31" s="15" t="inlineStr">
-        <is>
-          <t>Atun Dolores en agua con aceite 140g</t>
-        </is>
-      </c>
-      <c r="C31" s="15" t="inlineStr">
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>6307034</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>ACT II MANTEQUILLA OPTIMUS 6-14/80 GR (PALOMITAS)</t>
+        </is>
+      </c>
+      <c r="C34" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>7501040009761</t>
-        </is>
-      </c>
-      <c r="B32" s="15" t="inlineStr">
-        <is>
-          <t>Salchicas FUD con pavo 266g</t>
-        </is>
-      </c>
-      <c r="C32" s="15" t="inlineStr">
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <t>6307035</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>ACT II EXTRAMANTEQUILLA OPTIMUS 6-14/80 GR (PALOMITAS)</t>
+        </is>
+      </c>
+      <c r="C35" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>7501003340122</t>
-        </is>
-      </c>
-      <c r="B33" s="15" t="inlineStr">
-        <is>
-          <t>Mayonesa McCormik 190g</t>
-        </is>
-      </c>
-      <c r="C33" s="15" t="inlineStr">
+    <row r="36">
+      <c r="A36" s="16" t="inlineStr">
+        <is>
+          <t>6307315</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ACT II MANTEQUILLA PACK 12-3-90 GR </t>
+        </is>
+      </c>
+      <c r="C36" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>7702535002469</t>
-        </is>
-      </c>
-      <c r="B34" s="15" t="inlineStr">
-        <is>
-          <t>Jugo del Valle Kids de 200 ml c/u</t>
-        </is>
-      </c>
-      <c r="C34" s="15" t="inlineStr">
-        <is>
-          <t>Mililiros</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>7502227989975</t>
-        </is>
-      </c>
-      <c r="B35" s="15" t="inlineStr">
-        <is>
-          <t>Cafe Ricore  200g</t>
-        </is>
-      </c>
-      <c r="C35" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="inlineStr">
-        <is>
-          <t>7502226815053</t>
-        </is>
-      </c>
-      <c r="B36" s="15" t="inlineStr">
-        <is>
-          <t>Dulce Lucas muecas 24g</t>
-        </is>
-      </c>
-      <c r="C36" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
     <row r="37">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>7503025355757</t>
-        </is>
-      </c>
-      <c r="B37" s="15" t="inlineStr">
-        <is>
-          <t>Arroz medio grano Cies 900g</t>
-        </is>
-      </c>
-      <c r="C37" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
+      <c r="A37" s="16" t="inlineStr">
+        <is>
+          <t>9982824</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHEETOS 6-10/44GRS PACK </t>
+        </is>
+      </c>
+      <c r="C37" s="15" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t>7501040090967</t>
-        </is>
-      </c>
-      <c r="B38" s="15" t="inlineStr">
-        <is>
-          <t>Yoghurt natural Yoplait 442g</t>
+      <c r="A38" s="8" t="inlineStr">
+        <is>
+          <t>7501000651375</t>
+        </is>
+      </c>
+      <c r="B38" s="9" t="inlineStr">
+        <is>
+          <t>Galletas con malvavisco y cobertura sabor chocolate (mamut)</t>
         </is>
       </c>
       <c r="C38" s="15" t="inlineStr">
@@ -1117,12 +1113,12 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>7502261257856</t>
-        </is>
-      </c>
-      <c r="B39" s="15" t="inlineStr">
-        <is>
-          <t>Crema blanca crema 450g</t>
+          <t>7501000153107</t>
+        </is>
+      </c>
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>Gansito</t>
         </is>
       </c>
       <c r="C39" s="15" t="inlineStr">
@@ -1134,1159 +1130,857 @@
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>980022724</t>
+          <t>7501008051436</t>
         </is>
       </c>
       <c r="B40" s="15" t="inlineStr">
         <is>
-          <t>Cajeta Quemada Member's Mark 1.2 k</t>
+          <t>Barra de granola (Kellogg)</t>
         </is>
       </c>
       <c r="C40" s="15" t="inlineStr">
         <is>
-          <t>kilogramos</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="16" t="inlineStr">
-        <is>
-          <t>-0-0-0931305</t>
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>7501008051207</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
         <is>
-          <t>Frijol Verde Valle Flor de Mayo 2.5 kg</t>
+          <t>Barra suave con relleno sabor a frutos rojos (Kelloggs)</t>
         </is>
       </c>
       <c r="C41" s="15" t="inlineStr">
         <is>
-          <t>kilogramos</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="16" t="inlineStr">
-        <is>
-          <t>-0-0-0-358602</t>
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>7622210427106</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>Polvo para Preparar Bebida Gatorade Rehidratante 2.38 kg</t>
+          <t>Halls</t>
         </is>
       </c>
       <c r="C42" s="15" t="inlineStr">
         <is>
-          <t>kilogramos</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="16" t="inlineStr">
-        <is>
-          <t>4760413</t>
-        </is>
-      </c>
-      <c r="B43" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DORITOS 5 - 10 /54 GRS PACK </t>
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>7506309837239</t>
+        </is>
+      </c>
+      <c r="B43" s="15" t="inlineStr">
+        <is>
+          <t>Crema para peinar PANTENE</t>
         </is>
       </c>
       <c r="C43" s="15" t="inlineStr">
         <is>
+          <t xml:space="preserve">Miligramos </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>7622210572684</t>
+        </is>
+      </c>
+      <c r="B44" s="15" t="inlineStr">
+        <is>
+          <t>TANG</t>
+        </is>
+      </c>
+      <c r="C44" s="15" t="inlineStr">
+        <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="16" t="inlineStr">
-        <is>
-          <t>9987980</t>
-        </is>
-      </c>
-      <c r="B44" s="6" t="inlineStr">
-        <is>
-          <t>MAXI BOTANA INTENSOS TOTIS 40-85GR</t>
-        </is>
-      </c>
-      <c r="C44" s="15" t="inlineStr">
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>7501055307906</t>
+        </is>
+      </c>
+      <c r="B45" s="15" t="inlineStr">
+        <is>
+          <t>Ciel purificada</t>
+        </is>
+      </c>
+      <c r="C45" s="15" t="inlineStr">
+        <is>
+          <t>litros</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>7506192506571</t>
+        </is>
+      </c>
+      <c r="B46" s="15" t="inlineStr">
+        <is>
+          <t>eGo ATTRACTION</t>
+        </is>
+      </c>
+      <c r="C46" s="15" t="inlineStr">
+        <is>
+          <t>miligramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>7509546074016</t>
+        </is>
+      </c>
+      <c r="B47" s="15" t="inlineStr">
+        <is>
+          <t>Colgate Triple Acción</t>
+        </is>
+      </c>
+      <c r="C47" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="16" t="inlineStr">
-        <is>
-          <t>9987979</t>
-        </is>
-      </c>
-      <c r="B45" s="6" t="inlineStr">
-        <is>
-          <t>BOTANA TOTOPOS NACHO TOTIS 40-120GR</t>
-        </is>
-      </c>
-      <c r="C45" s="15" t="inlineStr">
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>7501000912803</t>
+        </is>
+      </c>
+      <c r="B48" s="15" t="inlineStr">
+        <is>
+          <t>Nescafe clásico</t>
+        </is>
+      </c>
+      <c r="C48" s="15" t="inlineStr">
         <is>
           <t>Gramos</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="16" t="inlineStr">
-        <is>
-          <t>9987977</t>
-        </is>
-      </c>
-      <c r="B46" s="6" t="inlineStr">
-        <is>
-          <t>BOTANAS TOTIS TOP´S SALSA NEGRA 8-10/52 GR</t>
-        </is>
-      </c>
-      <c r="C46" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="16" t="inlineStr">
-        <is>
-          <t>4760398</t>
-        </is>
-      </c>
-      <c r="B47" s="5" t="inlineStr">
-        <is>
-          <t>BOTANA DORITOS PACK 1-30 PZ</t>
-        </is>
-      </c>
-      <c r="C47" s="15" t="inlineStr">
-        <is>
-          <t>Pieza</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="16" t="inlineStr">
-        <is>
-          <t>4761205</t>
-        </is>
-      </c>
-      <c r="B48" s="6" t="inlineStr">
-        <is>
-          <t>BOTANA SABRISURTIDO SABRITAS 1-35 PZ</t>
-        </is>
-      </c>
-      <c r="C48" s="15" t="inlineStr">
-        <is>
-          <t>Piezas</t>
-        </is>
-      </c>
-    </row>
     <row r="49">
-      <c r="A49" s="16" t="inlineStr">
-        <is>
-          <t>4761234</t>
-        </is>
-      </c>
-      <c r="B49" s="5" t="inlineStr">
-        <is>
-          <t>BOTANA SABRIMAYOREO SABRITAS 1-50 PZ</t>
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>7503002541753</t>
+        </is>
+      </c>
+      <c r="B49" s="15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Agua purificada vie </t>
         </is>
       </c>
       <c r="C49" s="15" t="inlineStr">
         <is>
-          <t>Piezas</t>
+          <t xml:space="preserve">Litros </t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="16" t="inlineStr">
-        <is>
-          <t>6307033</t>
-        </is>
-      </c>
-      <c r="B50" s="6" t="inlineStr">
-        <is>
-          <t>ACT II NATURAL OPTIMUS 6-14/80 GR (PALOMITAS)</t>
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>7501017006021</t>
+        </is>
+      </c>
+      <c r="B50" s="15" t="inlineStr">
+        <is>
+          <t>chipotle adobados la costeña l05g</t>
         </is>
       </c>
       <c r="C50" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t xml:space="preserve">gramos </t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="7" t="inlineStr">
-        <is>
-          <t>6307034</t>
-        </is>
-      </c>
-      <c r="B51" s="6" t="inlineStr">
-        <is>
-          <t>ACT II MANTEQUILLA OPTIMUS 6-14/80 GR (PALOMITAS)</t>
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>7501003124241</t>
+        </is>
+      </c>
+      <c r="B51" s="15" t="inlineStr">
+        <is>
+          <t>garnos de elote herdez 400g</t>
         </is>
       </c>
       <c r="C51" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>gramos</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="7" t="inlineStr">
-        <is>
-          <t>6307035</t>
-        </is>
-      </c>
-      <c r="B52" s="6" t="inlineStr">
-        <is>
-          <t>ACT II EXTRAMANTEQUILLA OPTIMUS 6-14/80 GR (PALOMITAS)</t>
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>7501020560695</t>
+        </is>
+      </c>
+      <c r="B52" s="15" t="inlineStr">
+        <is>
+          <t>borel plus 1L</t>
         </is>
       </c>
       <c r="C52" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>litros</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="16" t="inlineStr">
-        <is>
-          <t>6307315</t>
-        </is>
-      </c>
-      <c r="B53" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ACT II MANTEQUILLA PACK 12-3-90 GR </t>
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>7501000111855</t>
+        </is>
+      </c>
+      <c r="B53" s="15" t="inlineStr">
+        <is>
+          <t>pan molido bimbo 190g</t>
         </is>
       </c>
       <c r="C53" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t xml:space="preserve">gramos </t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="16" t="inlineStr">
-        <is>
-          <t>9982824</t>
-        </is>
-      </c>
-      <c r="B54" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CHEETOS 6-10/44GRS PACK </t>
-        </is>
-      </c>
-      <c r="C54" s="15" t="n"/>
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>7501054500254</t>
+        </is>
+      </c>
+      <c r="B54" s="15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nívea crema corporal </t>
+        </is>
+      </c>
+      <c r="C54" s="15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mililitros </t>
+        </is>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="8" t="inlineStr">
-        <is>
-          <t>7501000651375</t>
-        </is>
-      </c>
-      <c r="B55" s="9" t="inlineStr">
-        <is>
-          <t>Galletas con malvavisco y cobertura sabor chocolate (mamut)</t>
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>7501055909520</t>
+        </is>
+      </c>
+      <c r="B55" s="11" t="inlineStr">
+        <is>
+          <t>crema alpura acidificada 200ml</t>
         </is>
       </c>
       <c r="C55" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>mililitros</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>7501000153107</t>
-        </is>
-      </c>
-      <c r="B56" s="10" t="inlineStr">
-        <is>
-          <t>Gansito</t>
+          <t>7503006897597</t>
+        </is>
+      </c>
+      <c r="B56" s="15" t="inlineStr">
+        <is>
+          <t>Refresco Jarritos 2Lt uva</t>
         </is>
       </c>
       <c r="C56" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>litros</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>7501008051436</t>
+          <t>7501000157075</t>
         </is>
       </c>
       <c r="B57" s="15" t="inlineStr">
         <is>
-          <t>Barra de granola (Kellogg)</t>
+          <t>Tostadas Milpa Real Onduladas360g</t>
         </is>
       </c>
       <c r="C57" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>gramos</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>7501008051207</t>
+          <t>7501058652690</t>
         </is>
       </c>
       <c r="B58" s="15" t="inlineStr">
         <is>
-          <t>Barra suave con relleno sabor a frutos rojos (Kelloggs)</t>
+          <t>Cereal Nestle Nesquik Sabor Chocolate 620g</t>
         </is>
       </c>
       <c r="C58" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>gramos</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>7622210427106</t>
+          <t>7501008025635</t>
         </is>
       </c>
       <c r="B59" s="15" t="inlineStr">
         <is>
-          <t>Halls</t>
+          <t>Barras Special Kelloggs Sabor Chocolate 200g</t>
         </is>
       </c>
       <c r="C59" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>gramos</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>7506309837239</t>
+          <t>7501011130272</t>
         </is>
       </c>
       <c r="B60" s="15" t="inlineStr">
         <is>
-          <t>Crema para peinar PANTENE</t>
+          <t>Doritos xtra-Flamin'hot</t>
         </is>
       </c>
       <c r="C60" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Miligramos </t>
+          <t>pieza</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>7622210572684</t>
+          <t>738545020015</t>
         </is>
       </c>
       <c r="B61" s="15" t="inlineStr">
         <is>
-          <t>TANG</t>
+          <t xml:space="preserve">Chamoy Mega Original </t>
         </is>
       </c>
       <c r="C61" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t>gramos</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>7501055307906</t>
+          <t>7501125116810</t>
         </is>
       </c>
       <c r="B62" s="15" t="inlineStr">
         <is>
-          <t>Ciel purificada</t>
+          <t xml:space="preserve">Agrifen, antigripal </t>
         </is>
       </c>
       <c r="C62" s="15" t="inlineStr">
         <is>
-          <t>litros</t>
+          <t>Miligramos</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>7506192506571</t>
+          <t>75062576</t>
         </is>
       </c>
       <c r="B63" s="15" t="inlineStr">
         <is>
-          <t>eGo ATTRACTION</t>
+          <t>Alka- seltzer</t>
         </is>
       </c>
       <c r="C63" s="15" t="inlineStr">
         <is>
-          <t>miligramos</t>
+          <t xml:space="preserve">Miligramos </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>7509546074016</t>
+          <t>7506495000547</t>
         </is>
       </c>
       <c r="B64" s="15" t="inlineStr">
         <is>
-          <t>Colgate Triple Acción</t>
+          <t xml:space="preserve">Hisopos de algodón </t>
         </is>
       </c>
       <c r="C64" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t xml:space="preserve">Piezas </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>7501000912803</t>
+          <t>4005900499257</t>
         </is>
       </c>
       <c r="B65" s="15" t="inlineStr">
         <is>
-          <t>Nescafe clásico</t>
+          <t>Agua micelar nivea</t>
         </is>
       </c>
       <c r="C65" s="15" t="inlineStr">
         <is>
-          <t>Gramos</t>
+          <t xml:space="preserve">Mililitros </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>7503002541753</t>
+          <t>757528012670</t>
         </is>
       </c>
       <c r="B66" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Agua purificada vie </t>
+          <t>Takis paleta fuego 24g</t>
         </is>
       </c>
       <c r="C66" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Litros </t>
+          <t xml:space="preserve">pieza </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>7501017006021</t>
+          <t>852933008352</t>
         </is>
       </c>
       <c r="B67" s="15" t="inlineStr">
         <is>
-          <t>chipotle adobados la costeña l05g</t>
+          <t xml:space="preserve">Women's multi vitamins </t>
         </is>
       </c>
       <c r="C67" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">gramos </t>
+          <t xml:space="preserve">Pieza </t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="inlineStr">
-        <is>
-          <t>7501003124241</t>
+      <c r="A68" s="12" t="inlineStr">
+        <is>
+          <t>19428</t>
         </is>
       </c>
       <c r="B68" s="15" t="inlineStr">
         <is>
-          <t>garnos de elote herdez 400g</t>
+          <t>Bebida Energética Volt Sabor Guaraná 473 Ml</t>
         </is>
       </c>
       <c r="C68" s="15" t="inlineStr">
         <is>
-          <t>gramos</t>
+          <t xml:space="preserve">Mililitros </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>7501020560695</t>
+          <t>7500326150999</t>
         </is>
       </c>
       <c r="B69" s="15" t="inlineStr">
         <is>
-          <t>borel plus 1L</t>
+          <t xml:space="preserve">Seltz vitaminas </t>
         </is>
       </c>
       <c r="C69" s="15" t="inlineStr">
         <is>
-          <t>litros</t>
+          <t xml:space="preserve">Miligramos </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>7501079011117</t>
+          <t>769836</t>
         </is>
       </c>
       <c r="B70" s="15" t="inlineStr">
         <is>
-          <t>italpasta 200g</t>
+          <t>Amper Bebida Energizante Energy 473 ml</t>
         </is>
       </c>
       <c r="C70" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">gramos </t>
+          <t xml:space="preserve">Mililitros </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>7501000111855</t>
+          <t>7501000116447</t>
         </is>
       </c>
       <c r="B71" s="15" t="inlineStr">
         <is>
-          <t>pan molido bimbo 190g</t>
+          <t>Brant Frut</t>
         </is>
       </c>
       <c r="C71" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">gramos </t>
+          <t xml:space="preserve">Gramos </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>7501054500254</t>
+          <t>633148100013</t>
         </is>
       </c>
       <c r="B72" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nívea crema corporal </t>
+          <t>tajín clásico 142g</t>
         </is>
       </c>
       <c r="C72" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mililitros </t>
+          <t xml:space="preserve">Gramos </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>7501055909520</t>
-        </is>
-      </c>
-      <c r="B73" s="11" t="inlineStr">
-        <is>
-          <t>crema alpura acidificada 200ml</t>
+          <t>7501030467090</t>
+        </is>
+      </c>
+      <c r="B73" s="15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pan Bimbo cero </t>
         </is>
       </c>
       <c r="C73" s="15" t="inlineStr">
         <is>
-          <t>mililitros</t>
+          <t xml:space="preserve">Gramos </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>7503006897597</t>
+          <t>7501761847970</t>
         </is>
       </c>
       <c r="B74" s="15" t="inlineStr">
         <is>
-          <t>Refresco Jarritos 2Lt uva</t>
+          <t xml:space="preserve">Barras con avena integral Stila </t>
         </is>
       </c>
       <c r="C74" s="15" t="inlineStr">
         <is>
-          <t>litros</t>
+          <t xml:space="preserve">Piezas </t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>7501000157075</t>
+          <t>7501943466357</t>
         </is>
       </c>
       <c r="B75" s="15" t="inlineStr">
         <is>
-          <t>Tostadas Milpa Real Onduladas360g</t>
+          <t xml:space="preserve">Pétalo servilletas de papel </t>
         </is>
       </c>
       <c r="C75" s="15" t="inlineStr">
         <is>
-          <t>gramos</t>
+          <t xml:space="preserve">Piezas </t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="inlineStr">
-        <is>
-          <t>7501058652690</t>
-        </is>
-      </c>
-      <c r="B76" s="15" t="inlineStr">
-        <is>
-          <t>Cereal Nestle Nesquik Sabor Chocolate 620g</t>
+      <c r="A76" s="13" t="inlineStr">
+        <is>
+          <t>725181105015</t>
+        </is>
+      </c>
+      <c r="B76" s="14" t="inlineStr">
+        <is>
+          <t>Skwinkles Clásicos Mars</t>
         </is>
       </c>
       <c r="C76" s="15" t="inlineStr">
         <is>
-          <t>gramos</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>7501008025635</t>
+          <t>658480001255</t>
         </is>
       </c>
       <c r="B77" s="15" t="inlineStr">
         <is>
-          <t>Barras Special Kelloggs Sabor Chocolate 200g</t>
+          <t xml:space="preserve">Salmas sanissimo </t>
         </is>
       </c>
       <c r="C77" s="15" t="inlineStr">
         <is>
-          <t>gramos</t>
+          <t xml:space="preserve">Gramos </t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="inlineStr">
-        <is>
-          <t>7501011130272</t>
-        </is>
-      </c>
-      <c r="B78" s="15" t="inlineStr">
-        <is>
-          <t>Doritos xtra-Flamin'hot</t>
+      <c r="A78" s="13" t="inlineStr">
+        <is>
+          <t>7501055321681</t>
+        </is>
+      </c>
+      <c r="B78" s="14" t="inlineStr">
+        <is>
+          <t>Coca Cola Sin Azúcar - 2.5 L</t>
         </is>
       </c>
       <c r="C78" s="15" t="inlineStr">
         <is>
-          <t>pieza</t>
+          <t>Litros</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>738545020015</t>
+          <t>7502238610226</t>
         </is>
       </c>
       <c r="B79" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chamoy Mega Original </t>
+          <t xml:space="preserve">Fun fun cucharas desechables </t>
         </is>
       </c>
       <c r="C79" s="15" t="inlineStr">
         <is>
-          <t>gramos</t>
+          <t xml:space="preserve">Piezas </t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="inlineStr">
-        <is>
-          <t>7501125116810</t>
-        </is>
-      </c>
-      <c r="B80" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Agrifen, antigripal </t>
+      <c r="A80" s="13" t="inlineStr">
+        <is>
+          <t>7501677921511</t>
+        </is>
+      </c>
+      <c r="B80" s="14" t="inlineStr">
+        <is>
+          <t>Kipi Bofitos</t>
         </is>
       </c>
       <c r="C80" s="15" t="inlineStr">
         <is>
-          <t>Miligramos</t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>75062576</t>
+          <t>75030332949123</t>
         </is>
       </c>
       <c r="B81" s="15" t="inlineStr">
         <is>
-          <t>Alka- seltzer</t>
+          <t xml:space="preserve">Leggs surtido de té </t>
         </is>
       </c>
       <c r="C81" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Miligramos </t>
+          <t xml:space="preserve">Piezas </t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="inlineStr">
-        <is>
-          <t>7506495000547</t>
-        </is>
-      </c>
-      <c r="B82" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hisopos de algodón </t>
+      <c r="A82" s="13" t="inlineStr">
+        <is>
+          <t>8000500267035</t>
+        </is>
+      </c>
+      <c r="B82" s="14" t="inlineStr">
+        <is>
+          <t>Kinder Délice - 39 g</t>
         </is>
       </c>
       <c r="C82" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Piezas </t>
+          <t xml:space="preserve">Gramos </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>4005900499257</t>
+          <t>7500478007639</t>
         </is>
       </c>
       <c r="B83" s="15" t="inlineStr">
         <is>
-          <t>Agua micelar nivea</t>
+          <t>Sabritas Receta Crujiente Flamin Hot 70 g Bolzaza</t>
         </is>
       </c>
       <c r="C83" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mililitros </t>
+          <t xml:space="preserve">pieza </t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t>757528012670</t>
-        </is>
-      </c>
-      <c r="B84" s="15" t="inlineStr">
-        <is>
-          <t>Takis paleta fuego 24g</t>
+      <c r="A84" s="13" t="inlineStr">
+        <is>
+          <t>7501011115590</t>
+        </is>
+      </c>
+      <c r="B84" s="14" t="inlineStr">
+        <is>
+          <t>Sabritas Crema y Especias - 170 g</t>
         </is>
       </c>
       <c r="C84" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">pieza </t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>852933008352</t>
+          <t>7501007531847</t>
         </is>
       </c>
       <c r="B85" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Women's multi vitamins </t>
+          <t>Listerine 250 ml</t>
         </is>
       </c>
       <c r="C85" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pieza </t>
+          <t>Litros</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="12" t="inlineStr">
-        <is>
-          <t>19428</t>
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>75063006247505</t>
         </is>
       </c>
       <c r="B86" s="15" t="inlineStr">
         <is>
-          <t>Bebida Energética Volt Sabor Guaraná 473 Ml</t>
+          <t>Gel ego</t>
         </is>
       </c>
       <c r="C86" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mililitros </t>
+          <t>Litros</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>7500326150999</t>
+          <t>7506306245686</t>
         </is>
       </c>
       <c r="B87" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Seltz vitaminas </t>
+          <t>Axe epic fresh</t>
         </is>
       </c>
       <c r="C87" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Miligramos </t>
+          <t xml:space="preserve">Litros </t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>769836</t>
+          <t>7501052472447</t>
         </is>
       </c>
       <c r="B88" s="15" t="inlineStr">
         <is>
-          <t>Amper Bebida Energizante Energy 473 ml</t>
+          <t>Clemente jacques catsup 320 gr</t>
         </is>
       </c>
       <c r="C88" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mililitros </t>
+          <t>Gramos</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>7501000116447</t>
+          <t>7503002541821</t>
         </is>
       </c>
       <c r="B89" s="15" t="inlineStr">
         <is>
-          <t>Brant Frut</t>
+          <t>Agua vie 1L</t>
         </is>
       </c>
       <c r="C89" s="15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gramos </t>
+          <t xml:space="preserve">Litros </t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="inlineStr">
-        <is>
-          <t>633148100013</t>
-        </is>
-      </c>
-      <c r="B90" s="15" t="inlineStr">
-        <is>
-          <t>tajín clásico 142g</t>
-        </is>
-      </c>
-      <c r="C90" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Gramos </t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="2" t="inlineStr">
-        <is>
-          <t>7501030467090</t>
-        </is>
-      </c>
-      <c r="B91" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pan Bimbo cero </t>
-        </is>
-      </c>
-      <c r="C91" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Gramos </t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="2" t="inlineStr">
-        <is>
-          <t>7501761847970</t>
-        </is>
-      </c>
-      <c r="B92" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Barras con avena integral Stila </t>
-        </is>
-      </c>
-      <c r="C92" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Piezas </t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="2" t="inlineStr">
-        <is>
-          <t>7501943466357</t>
-        </is>
-      </c>
-      <c r="B93" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pétalo servilletas de papel </t>
-        </is>
-      </c>
-      <c r="C93" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Piezas </t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="13" t="inlineStr">
-        <is>
-          <t>725181105015</t>
-        </is>
-      </c>
-      <c r="B94" s="14" t="inlineStr">
-        <is>
-          <t>Skwinkles Clásicos Mars</t>
-        </is>
-      </c>
-      <c r="C94" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="2" t="inlineStr">
-        <is>
-          <t>658480001255</t>
-        </is>
-      </c>
-      <c r="B95" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Salmas sanissimo </t>
-        </is>
-      </c>
-      <c r="C95" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Gramos </t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="13" t="inlineStr">
-        <is>
-          <t>7501055321681</t>
-        </is>
-      </c>
-      <c r="B96" s="14" t="inlineStr">
-        <is>
-          <t>Coca Cola Sin Azúcar - 2.5 L</t>
-        </is>
-      </c>
-      <c r="C96" s="15" t="inlineStr">
-        <is>
-          <t>Litros</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="2" t="inlineStr">
-        <is>
-          <t>7502238610226</t>
-        </is>
-      </c>
-      <c r="B97" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fun fun cucharas desechables </t>
-        </is>
-      </c>
-      <c r="C97" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Piezas </t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="13" t="inlineStr">
-        <is>
-          <t>7501677921511</t>
-        </is>
-      </c>
-      <c r="B98" s="14" t="inlineStr">
-        <is>
-          <t>Kipi Bofitos</t>
-        </is>
-      </c>
-      <c r="C98" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="2" t="inlineStr">
-        <is>
-          <t>75030332949123</t>
-        </is>
-      </c>
-      <c r="B99" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Leggs surtido de té </t>
-        </is>
-      </c>
-      <c r="C99" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Piezas </t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="13" t="inlineStr">
-        <is>
-          <t>8000500267035</t>
-        </is>
-      </c>
-      <c r="B100" s="14" t="inlineStr">
-        <is>
-          <t>Kinder Délice - 39 g</t>
-        </is>
-      </c>
-      <c r="C100" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Gramos </t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="2" t="inlineStr">
-        <is>
-          <t>7500478007639</t>
-        </is>
-      </c>
-      <c r="B101" s="15" t="inlineStr">
-        <is>
-          <t>Sabritas Receta Crujiente Flamin Hot 70 g Bolzaza</t>
-        </is>
-      </c>
-      <c r="C101" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">pieza </t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="13" t="inlineStr">
-        <is>
-          <t>7501011115590</t>
-        </is>
-      </c>
-      <c r="B102" s="14" t="inlineStr">
-        <is>
-          <t>Sabritas Crema y Especias - 170 g</t>
-        </is>
-      </c>
-      <c r="C102" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="2" t="inlineStr">
-        <is>
-          <t>7501007531847</t>
-        </is>
-      </c>
-      <c r="B103" s="15" t="inlineStr">
-        <is>
-          <t>Listerine 250 ml</t>
-        </is>
-      </c>
-      <c r="C103" s="15" t="inlineStr">
-        <is>
-          <t>Litros</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="2" t="inlineStr">
-        <is>
-          <t>75063006247505</t>
-        </is>
-      </c>
-      <c r="B104" s="15" t="inlineStr">
-        <is>
-          <t>Gel ego</t>
-        </is>
-      </c>
-      <c r="C104" s="15" t="inlineStr">
-        <is>
-          <t>Litros</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="2" t="inlineStr">
-        <is>
-          <t>7506306245686</t>
-        </is>
-      </c>
-      <c r="B105" s="15" t="inlineStr">
-        <is>
-          <t>Axe epic fresh</t>
-        </is>
-      </c>
-      <c r="C105" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Litros </t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="2" t="inlineStr">
-        <is>
-          <t>7501052472447</t>
-        </is>
-      </c>
-      <c r="B106" s="15" t="inlineStr">
-        <is>
-          <t>Clemente jacques catsup 320 gr</t>
-        </is>
-      </c>
-      <c r="C106" s="15" t="inlineStr">
-        <is>
-          <t>Gramos</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="2" t="inlineStr">
-        <is>
-          <t>7503002541821</t>
-        </is>
-      </c>
-      <c r="B107" s="15" t="inlineStr">
-        <is>
-          <t>Agua vie 1L</t>
-        </is>
-      </c>
-      <c r="C107" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Litros </t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="15" t="n"/>
-      <c r="B108" s="15" t="n"/>
-      <c r="C108" s="15" t="n"/>
+      <c r="A90" s="15" t="n"/>
+      <c r="B90" s="15" t="n"/>
+      <c r="C90" s="15" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2299,7 +1993,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3004,7 +2698,6 @@
         </is>
       </c>
     </row>
-    <row r="23"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>